<commit_message>
all data was swapped for years 2010-2018 data
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">Annual Counts from NPS Survey</t>
   </si>
@@ -23,6 +23,30 @@
   </si>
   <si>
     <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017</t>
   </si>
   <si>
     <t xml:space="preserve">2018</t>
@@ -240,7 +264,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane state="frozen" xSplit="1" ySplit="2" topLeftCell="B3"/>
@@ -250,6 +274,14 @@
   <cols>
     <col min="1" max="1" customWidth="1" width="19.9296875"/>
     <col min="2" max="2" customWidth="1" width="19.9296875"/>
+    <col min="3" max="3" customWidth="1" width="19.9296875"/>
+    <col min="4" max="4" customWidth="1" width="19.9296875"/>
+    <col min="5" max="5" customWidth="1" width="19.9296875"/>
+    <col min="6" max="6" customWidth="1" width="19.9296875"/>
+    <col min="7" max="7" customWidth="1" width="19.9296875"/>
+    <col min="8" max="8" customWidth="1" width="19.9296875"/>
+    <col min="9" max="9" customWidth="1" width="19.9296875"/>
+    <col min="10" max="10" customWidth="1" width="19.9296875"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -259,6 +291,22 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1">
+             </c>
+      <c r="D1">
+             </c>
+      <c r="E1">
+             </c>
+      <c r="F1">
+             </c>
+      <c r="G1">
+             </c>
+      <c r="H1">
+             </c>
+      <c r="I1">
+             </c>
+      <c r="J1">
+             </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -267,408 +315,1635 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" t="n">
+        <v>5391</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5597</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5633</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5081</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5794</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5338</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4434</v>
+      </c>
+      <c r="I3" t="n">
+        <v>4399</v>
+      </c>
+      <c r="J3" t="n">
         <v>4380</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B4" t="n">
+        <v>31764</v>
+      </c>
+      <c r="C4" t="n">
+        <v>32270</v>
+      </c>
+      <c r="D4" t="n">
+        <v>32431</v>
+      </c>
+      <c r="E4" t="n">
+        <v>32381</v>
+      </c>
+      <c r="F4" t="n">
+        <v>31771</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30810</v>
+      </c>
+      <c r="H4" t="n">
+        <v>28883</v>
+      </c>
+      <c r="I4" t="n">
+        <v>27608</v>
+      </c>
+      <c r="J4" t="n">
         <v>26841</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5" t="n">
+        <v>16204</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16108</v>
+      </c>
+      <c r="D5" t="n">
+        <v>14654</v>
+      </c>
+      <c r="E5" t="n">
+        <v>17235</v>
+      </c>
+      <c r="F5" t="n">
+        <v>17874</v>
+      </c>
+      <c r="G5" t="n">
+        <v>17707</v>
+      </c>
+      <c r="H5" t="n">
+        <v>17537</v>
+      </c>
+      <c r="I5" t="n">
+        <v>18070</v>
+      </c>
+      <c r="J5" t="n">
         <v>17799</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6" t="n">
+        <v>40209</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40020</v>
+      </c>
+      <c r="D6" t="n">
+        <v>40080</v>
+      </c>
+      <c r="E6" t="n">
+        <v>41177</v>
+      </c>
+      <c r="F6" t="n">
+        <v>42259</v>
+      </c>
+      <c r="G6" t="n">
+        <v>42719</v>
+      </c>
+      <c r="H6" t="n">
+        <v>42320</v>
+      </c>
+      <c r="I6" t="n">
+        <v>42030</v>
+      </c>
+      <c r="J6" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B7" t="n">
+        <v>165062</v>
+      </c>
+      <c r="C7" t="n">
+        <v>149569</v>
+      </c>
+      <c r="D7" t="n">
+        <v>134534</v>
+      </c>
+      <c r="E7" t="n">
+        <v>135981</v>
+      </c>
+      <c r="F7" t="n">
+        <v>136085</v>
+      </c>
+      <c r="G7" t="n">
+        <v>129593</v>
+      </c>
+      <c r="H7" t="n">
+        <v>130084</v>
+      </c>
+      <c r="I7" t="n">
+        <v>131039</v>
+      </c>
+      <c r="J7" t="n">
         <v>128625</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B8" t="n">
+        <v>22815</v>
+      </c>
+      <c r="C8" t="n">
+        <v>21978</v>
+      </c>
+      <c r="D8" t="n">
+        <v>20462</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20371</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20646</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20041</v>
+      </c>
+      <c r="H8" t="n">
+        <v>19981</v>
+      </c>
+      <c r="I8" t="n">
+        <v>19946</v>
+      </c>
+      <c r="J8" t="n">
         <v>20372</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B9" t="n">
+        <v>19321</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18324</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17530</v>
+      </c>
+      <c r="E9" t="n">
+        <v>17563</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16636</v>
+      </c>
+      <c r="G9" t="n">
+        <v>15816</v>
+      </c>
+      <c r="H9" t="n">
+        <v>14957</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14040</v>
+      </c>
+      <c r="J9" t="n">
         <v>13681</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B10" t="n">
+        <v>6615</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6739</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6914</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7004</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6955</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6654</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6585</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6443</v>
+      </c>
+      <c r="J10" t="n">
         <v>6067</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B11" t="n">
+        <v>104306</v>
+      </c>
+      <c r="C11" t="n">
+        <v>103055</v>
+      </c>
+      <c r="D11" t="n">
+        <v>101930</v>
+      </c>
+      <c r="E11" t="n">
+        <v>103028</v>
+      </c>
+      <c r="F11" t="n">
+        <v>102870</v>
+      </c>
+      <c r="G11" t="n">
+        <v>101424</v>
+      </c>
+      <c r="H11" t="n">
+        <v>99974</v>
+      </c>
+      <c r="I11" t="n">
+        <v>98504</v>
+      </c>
+      <c r="J11" t="n">
         <v>97538</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B12" t="n">
+        <v>56432</v>
+      </c>
+      <c r="C12" t="n">
+        <v>55944</v>
+      </c>
+      <c r="D12" t="n">
+        <v>55457</v>
+      </c>
+      <c r="E12" t="n">
+        <v>54004</v>
+      </c>
+      <c r="F12" t="n">
+        <v>52949</v>
+      </c>
+      <c r="G12" t="n">
+        <v>52193</v>
+      </c>
+      <c r="H12" t="n">
+        <v>53627</v>
+      </c>
+      <c r="I12" t="n">
+        <v>53667</v>
+      </c>
+      <c r="J12" t="n">
         <v>53647</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B13" t="n">
+        <v>5912</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6037</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5831</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5632</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5866</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5879</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5602</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5630</v>
+      </c>
+      <c r="J13" t="n">
         <v>5375</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B14" t="n">
+        <v>9455</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9116</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8733</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8697</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8838</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8849</v>
+      </c>
+      <c r="H14" t="n">
+        <v>9031</v>
+      </c>
+      <c r="I14" t="n">
+        <v>9024</v>
+      </c>
+      <c r="J14" t="n">
         <v>9419</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B15" t="n">
+        <v>7431</v>
+      </c>
+      <c r="C15" t="n">
+        <v>7739</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7985</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8242</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8117</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8052</v>
+      </c>
+      <c r="H15" t="n">
+        <v>8252</v>
+      </c>
+      <c r="I15" t="n">
+        <v>8579</v>
+      </c>
+      <c r="J15" t="n">
         <v>8664</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B16" t="n">
+        <v>48418</v>
+      </c>
+      <c r="C16" t="n">
+        <v>48427</v>
+      </c>
+      <c r="D16" t="n">
+        <v>49348</v>
+      </c>
+      <c r="E16" t="n">
+        <v>48653</v>
+      </c>
+      <c r="F16" t="n">
+        <v>48278</v>
+      </c>
+      <c r="G16" t="n">
+        <v>46240</v>
+      </c>
+      <c r="H16" t="n">
+        <v>43657</v>
+      </c>
+      <c r="I16" t="n">
+        <v>41427</v>
+      </c>
+      <c r="J16" t="n">
         <v>39965</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B17" t="n">
+        <v>28028</v>
+      </c>
+      <c r="C17" t="n">
+        <v>28906</v>
+      </c>
+      <c r="D17" t="n">
+        <v>28831</v>
+      </c>
+      <c r="E17" t="n">
+        <v>29913</v>
+      </c>
+      <c r="F17" t="n">
+        <v>29271</v>
+      </c>
+      <c r="G17" t="n">
+        <v>27355</v>
+      </c>
+      <c r="H17" t="n">
+        <v>25546</v>
+      </c>
+      <c r="I17" t="n">
+        <v>26024</v>
+      </c>
+      <c r="J17" t="n">
         <v>26877</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B18" t="n">
+        <v>9051</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9327</v>
+      </c>
+      <c r="D18" t="n">
+        <v>9682</v>
+      </c>
+      <c r="E18" t="n">
+        <v>9763</v>
+      </c>
+      <c r="F18" t="n">
+        <v>9877</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9857</v>
+      </c>
+      <c r="H18" t="n">
+        <v>9920</v>
+      </c>
+      <c r="I18" t="n">
+        <v>10015</v>
+      </c>
+      <c r="J18" t="n">
         <v>10218</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B19" t="n">
+        <v>20544</v>
+      </c>
+      <c r="C19" t="n">
+        <v>21545</v>
+      </c>
+      <c r="D19" t="n">
+        <v>22110</v>
+      </c>
+      <c r="E19" t="n">
+        <v>21030</v>
+      </c>
+      <c r="F19" t="n">
+        <v>21657</v>
+      </c>
+      <c r="G19" t="n">
+        <v>21701</v>
+      </c>
+      <c r="H19" t="n">
+        <v>23022</v>
+      </c>
+      <c r="I19" t="n">
+        <v>23543</v>
+      </c>
+      <c r="J19" t="n">
         <v>23431</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B20" t="n">
+        <v>39445</v>
+      </c>
+      <c r="C20" t="n">
+        <v>39710</v>
+      </c>
+      <c r="D20" t="n">
+        <v>40172</v>
+      </c>
+      <c r="E20" t="n">
+        <v>39299</v>
+      </c>
+      <c r="F20" t="n">
+        <v>38030</v>
+      </c>
+      <c r="G20" t="n">
+        <v>36377</v>
+      </c>
+      <c r="H20" t="n">
+        <v>35682</v>
+      </c>
+      <c r="I20" t="n">
+        <v>33739</v>
+      </c>
+      <c r="J20" t="n">
         <v>32397</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B21" t="n">
+        <v>11313</v>
+      </c>
+      <c r="C21" t="n">
+        <v>11623</v>
+      </c>
+      <c r="D21" t="n">
+        <v>11308</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10950</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10713</v>
+      </c>
+      <c r="G21" t="n">
+        <v>9922</v>
+      </c>
+      <c r="H21" t="n">
+        <v>9403</v>
+      </c>
+      <c r="I21" t="n">
+        <v>9133</v>
+      </c>
+      <c r="J21" t="n">
         <v>8692</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B22" t="n">
+        <v>22645</v>
+      </c>
+      <c r="C22" t="n">
+        <v>22558</v>
+      </c>
+      <c r="D22" t="n">
+        <v>21522</v>
+      </c>
+      <c r="E22" t="n">
+        <v>21335</v>
+      </c>
+      <c r="F22" t="n">
+        <v>21011</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20764</v>
+      </c>
+      <c r="H22" t="n">
+        <v>19994</v>
+      </c>
+      <c r="I22" t="n">
+        <v>19367</v>
+      </c>
+      <c r="J22" t="n">
         <v>18856</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B23" t="n">
+        <v>2154</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2145</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2108</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2173</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2242</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2279</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2404</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2404</v>
+      </c>
+      <c r="J23" t="n">
         <v>2425</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B24" t="n">
+        <v>44165</v>
+      </c>
+      <c r="C24" t="n">
+        <v>42940</v>
+      </c>
+      <c r="D24" t="n">
+        <v>43636</v>
+      </c>
+      <c r="E24" t="n">
+        <v>43759</v>
+      </c>
+      <c r="F24" t="n">
+        <v>43390</v>
+      </c>
+      <c r="G24" t="n">
+        <v>42628</v>
+      </c>
+      <c r="H24" t="n">
+        <v>41122</v>
+      </c>
+      <c r="I24" t="n">
+        <v>39666</v>
+      </c>
+      <c r="J24" t="n">
         <v>38761</v>
       </c>
     </row>
     <row r="25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B25" t="n">
+        <v>9796</v>
+      </c>
+      <c r="C25" t="n">
+        <v>9800</v>
+      </c>
+      <c r="D25" t="n">
+        <v>9938</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10289</v>
+      </c>
+      <c r="F25" t="n">
+        <v>10637</v>
+      </c>
+      <c r="G25" t="n">
+        <v>10798</v>
+      </c>
+      <c r="H25" t="n">
+        <v>10592</v>
+      </c>
+      <c r="I25" t="n">
+        <v>10708</v>
+      </c>
+      <c r="J25" t="n">
         <v>10101</v>
       </c>
     </row>
     <row r="26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B26" t="n">
+        <v>30623</v>
+      </c>
+      <c r="C26" t="n">
+        <v>30833</v>
+      </c>
+      <c r="D26" t="n">
+        <v>31247</v>
+      </c>
+      <c r="E26" t="n">
+        <v>31537</v>
+      </c>
+      <c r="F26" t="n">
+        <v>31942</v>
+      </c>
+      <c r="G26" t="n">
+        <v>32330</v>
+      </c>
+      <c r="H26" t="n">
+        <v>32461</v>
+      </c>
+      <c r="I26" t="n">
+        <v>32601</v>
+      </c>
+      <c r="J26" t="n">
         <v>30369</v>
       </c>
     </row>
     <row r="27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B27" t="n">
+        <v>21067</v>
+      </c>
+      <c r="C27" t="n">
+        <v>21386</v>
+      </c>
+      <c r="D27" t="n">
+        <v>22319</v>
+      </c>
+      <c r="E27" t="n">
+        <v>21969</v>
+      </c>
+      <c r="F27" t="n">
+        <v>18793</v>
+      </c>
+      <c r="G27" t="n">
+        <v>18911</v>
+      </c>
+      <c r="H27" t="n">
+        <v>19192</v>
+      </c>
+      <c r="I27" t="n">
+        <v>19103</v>
+      </c>
+      <c r="J27" t="n">
         <v>19275</v>
       </c>
     </row>
     <row r="28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B28" t="n">
+        <v>3716</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3678</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3609</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3642</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3699</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3685</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3814</v>
+      </c>
+      <c r="I28" t="n">
+        <v>3698</v>
+      </c>
+      <c r="J28" t="n">
         <v>3765</v>
       </c>
     </row>
     <row r="29" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B29" t="n">
+        <v>40382</v>
+      </c>
+      <c r="C29" t="n">
+        <v>39440</v>
+      </c>
+      <c r="D29" t="n">
+        <v>37136</v>
+      </c>
+      <c r="E29" t="n">
+        <v>36922</v>
+      </c>
+      <c r="F29" t="n">
+        <v>37096</v>
+      </c>
+      <c r="G29" t="n">
+        <v>36617</v>
+      </c>
+      <c r="H29" t="n">
+        <v>35697</v>
+      </c>
+      <c r="I29" t="n">
+        <v>36394</v>
+      </c>
+      <c r="J29" t="n">
         <v>34899</v>
       </c>
     </row>
     <row r="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B30" t="n">
+        <v>1487</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1423</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1512</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1576</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1718</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1795</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1791</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1723</v>
+      </c>
+      <c r="J30" t="n">
         <v>1695</v>
       </c>
     </row>
     <row r="31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B31" t="n">
+        <v>4587</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4616</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4705</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5026</v>
+      </c>
+      <c r="F31" t="n">
+        <v>5441</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5372</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5302</v>
+      </c>
+      <c r="I31" t="n">
+        <v>5313</v>
+      </c>
+      <c r="J31" t="n">
         <v>5491</v>
       </c>
     </row>
     <row r="32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B32" t="n">
+        <v>2761</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2614</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2790</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3018</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2963</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2897</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2818</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2750</v>
+      </c>
+      <c r="J32" t="n">
         <v>2722</v>
       </c>
     </row>
     <row r="33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B33" t="n">
+        <v>25007</v>
+      </c>
+      <c r="C33" t="n">
+        <v>23834</v>
+      </c>
+      <c r="D33" t="n">
+        <v>23225</v>
+      </c>
+      <c r="E33" t="n">
+        <v>22452</v>
+      </c>
+      <c r="F33" t="n">
+        <v>21590</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20489</v>
+      </c>
+      <c r="H33" t="n">
+        <v>19786</v>
+      </c>
+      <c r="I33" t="n">
+        <v>19585</v>
+      </c>
+      <c r="J33" t="n">
         <v>19362</v>
       </c>
     </row>
     <row r="34" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B34" t="n">
+        <v>6763</v>
+      </c>
+      <c r="C34" t="n">
+        <v>6998</v>
+      </c>
+      <c r="D34" t="n">
+        <v>6727</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6931</v>
+      </c>
+      <c r="F34" t="n">
+        <v>7021</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7104</v>
+      </c>
+      <c r="H34" t="n">
+        <v>7055</v>
+      </c>
+      <c r="I34" t="n">
+        <v>7276</v>
+      </c>
+      <c r="J34" t="n">
         <v>7030</v>
       </c>
     </row>
     <row r="35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B35" t="n">
+        <v>12653</v>
+      </c>
+      <c r="C35" t="n">
+        <v>12778</v>
+      </c>
+      <c r="D35" t="n">
+        <v>12883</v>
+      </c>
+      <c r="E35" t="n">
+        <v>13056</v>
+      </c>
+      <c r="F35" t="n">
+        <v>12537</v>
+      </c>
+      <c r="G35" t="n">
+        <v>13071</v>
+      </c>
+      <c r="H35" t="n">
+        <v>13757</v>
+      </c>
+      <c r="I35" t="n">
+        <v>13721</v>
+      </c>
+      <c r="J35" t="n">
         <v>13641</v>
       </c>
     </row>
     <row r="36" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B36" t="n">
+        <v>56656</v>
+      </c>
+      <c r="C36" t="n">
+        <v>55436</v>
+      </c>
+      <c r="D36" t="n">
+        <v>54210</v>
+      </c>
+      <c r="E36" t="n">
+        <v>53550</v>
+      </c>
+      <c r="F36" t="n">
+        <v>52518</v>
+      </c>
+      <c r="G36" t="n">
+        <v>51727</v>
+      </c>
+      <c r="H36" t="n">
+        <v>50716</v>
+      </c>
+      <c r="I36" t="n">
+        <v>49461</v>
+      </c>
+      <c r="J36" t="n">
         <v>46636</v>
       </c>
     </row>
     <row r="37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B37" t="n">
+        <v>51712</v>
+      </c>
+      <c r="C37" t="n">
+        <v>50964</v>
+      </c>
+      <c r="D37" t="n">
+        <v>50876</v>
+      </c>
+      <c r="E37" t="n">
+        <v>51729</v>
+      </c>
+      <c r="F37" t="n">
+        <v>51519</v>
+      </c>
+      <c r="G37" t="n">
+        <v>52233</v>
+      </c>
+      <c r="H37" t="n">
+        <v>52175</v>
+      </c>
+      <c r="I37" t="n">
+        <v>51478</v>
+      </c>
+      <c r="J37" t="n">
         <v>50431</v>
       </c>
     </row>
     <row r="38" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B38" t="n">
+        <v>26252</v>
+      </c>
+      <c r="C38" t="n">
+        <v>25977</v>
+      </c>
+      <c r="D38" t="n">
+        <v>25225</v>
+      </c>
+      <c r="E38" t="n">
+        <v>27547</v>
+      </c>
+      <c r="F38" t="n">
+        <v>27650</v>
+      </c>
+      <c r="G38" t="n">
+        <v>28547</v>
+      </c>
+      <c r="H38" t="n">
+        <v>29916</v>
+      </c>
+      <c r="I38" t="n">
+        <v>28143</v>
+      </c>
+      <c r="J38" t="n">
         <v>26956</v>
       </c>
     </row>
     <row r="39" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B39" t="n">
+        <v>14876</v>
+      </c>
+      <c r="C39" t="n">
+        <v>14510</v>
+      </c>
+      <c r="D39" t="n">
+        <v>14840</v>
+      </c>
+      <c r="E39" t="n">
+        <v>15517</v>
+      </c>
+      <c r="F39" t="n">
+        <v>15075</v>
+      </c>
+      <c r="G39" t="n">
+        <v>15245</v>
+      </c>
+      <c r="H39" t="n">
+        <v>15166</v>
+      </c>
+      <c r="I39" t="n">
+        <v>15218</v>
+      </c>
+      <c r="J39" t="n">
         <v>15268</v>
       </c>
     </row>
     <row r="40" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B40" t="n">
+        <v>51264</v>
+      </c>
+      <c r="C40" t="n">
+        <v>51578</v>
+      </c>
+      <c r="D40" t="n">
+        <v>51125</v>
+      </c>
+      <c r="E40" t="n">
+        <v>51422</v>
+      </c>
+      <c r="F40" t="n">
+        <v>50694</v>
+      </c>
+      <c r="G40" t="n">
+        <v>49858</v>
+      </c>
+      <c r="H40" t="n">
+        <v>49244</v>
+      </c>
+      <c r="I40" t="n">
+        <v>48333</v>
+      </c>
+      <c r="J40" t="n">
         <v>47239</v>
       </c>
     </row>
     <row r="41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B41" t="n">
+        <v>3357</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3337</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3318</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3361</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3359</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3248</v>
+      </c>
+      <c r="H41" t="n">
+        <v>3103</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2861</v>
+      </c>
+      <c r="J41" t="n">
         <v>2767</v>
       </c>
     </row>
     <row r="42" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B42" t="n">
+        <v>23578</v>
+      </c>
+      <c r="C42" t="n">
+        <v>22914</v>
+      </c>
+      <c r="D42" t="n">
+        <v>22388</v>
+      </c>
+      <c r="E42" t="n">
+        <v>22060</v>
+      </c>
+      <c r="F42" t="n">
+        <v>21401</v>
+      </c>
+      <c r="G42" t="n">
+        <v>20929</v>
+      </c>
+      <c r="H42" t="n">
+        <v>20858</v>
+      </c>
+      <c r="I42" t="n">
+        <v>19906</v>
+      </c>
+      <c r="J42" t="n">
         <v>19033</v>
       </c>
     </row>
     <row r="43" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B43" t="n">
+        <v>3434</v>
+      </c>
+      <c r="C43" t="n">
+        <v>3535</v>
+      </c>
+      <c r="D43" t="n">
+        <v>3650</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3682</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3608</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3564</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3831</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3970</v>
+      </c>
+      <c r="J43" t="n">
         <v>3948</v>
       </c>
     </row>
     <row r="44" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B44" t="n">
+        <v>27451</v>
+      </c>
+      <c r="C44" t="n">
+        <v>28479</v>
+      </c>
+      <c r="D44" t="n">
+        <v>28411</v>
+      </c>
+      <c r="E44" t="n">
+        <v>28521</v>
+      </c>
+      <c r="F44" t="n">
+        <v>28769</v>
+      </c>
+      <c r="G44" t="n">
+        <v>28172</v>
+      </c>
+      <c r="H44" t="n">
+        <v>28203</v>
+      </c>
+      <c r="I44" t="n">
+        <v>28980</v>
+      </c>
+      <c r="J44" t="n">
         <v>26321</v>
       </c>
     </row>
     <row r="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B45" t="n">
+        <v>173649</v>
+      </c>
+      <c r="C45" t="n">
+        <v>172224</v>
+      </c>
+      <c r="D45" t="n">
+        <v>166372</v>
+      </c>
+      <c r="E45" t="n">
+        <v>168280</v>
+      </c>
+      <c r="F45" t="n">
+        <v>166043</v>
+      </c>
+      <c r="G45" t="n">
+        <v>163909</v>
+      </c>
+      <c r="H45" t="n">
+        <v>163703</v>
+      </c>
+      <c r="I45" t="n">
+        <v>162523</v>
+      </c>
+      <c r="J45" t="n">
         <v>163628</v>
       </c>
     </row>
     <row r="46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B46" t="n">
+        <v>6807</v>
+      </c>
+      <c r="C46" t="n">
+        <v>6879</v>
+      </c>
+      <c r="D46" t="n">
+        <v>6962</v>
+      </c>
+      <c r="E46" t="n">
+        <v>7077</v>
+      </c>
+      <c r="F46" t="n">
+        <v>7031</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6495</v>
+      </c>
+      <c r="H46" t="n">
+        <v>6175</v>
+      </c>
+      <c r="I46" t="n">
+        <v>6219</v>
+      </c>
+      <c r="J46" t="n">
         <v>6651</v>
       </c>
     </row>
     <row r="47" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B47" t="n">
+        <v>37638</v>
+      </c>
+      <c r="C47" t="n">
+        <v>38130</v>
+      </c>
+      <c r="D47" t="n">
+        <v>37044</v>
+      </c>
+      <c r="E47" t="n">
+        <v>36982</v>
+      </c>
+      <c r="F47" t="n">
+        <v>37544</v>
+      </c>
+      <c r="G47" t="n">
+        <v>38403</v>
+      </c>
+      <c r="H47" t="n">
+        <v>37813</v>
+      </c>
+      <c r="I47" t="n">
+        <v>37158</v>
+      </c>
+      <c r="J47" t="n">
         <v>36660</v>
       </c>
     </row>
     <row r="48" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B48" t="n">
+        <v>2079</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2053</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2034</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2078</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1979</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1750</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1735</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1546</v>
+      </c>
+      <c r="J48" t="n">
         <v>1659</v>
       </c>
     </row>
     <row r="49" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B49" t="n">
+        <v>18235</v>
+      </c>
+      <c r="C49" t="n">
+        <v>17847</v>
+      </c>
+      <c r="D49" t="n">
+        <v>17271</v>
+      </c>
+      <c r="E49" t="n">
+        <v>17984</v>
+      </c>
+      <c r="F49" t="n">
+        <v>18120</v>
+      </c>
+      <c r="G49" t="n">
+        <v>18284</v>
+      </c>
+      <c r="H49" t="n">
+        <v>19104</v>
+      </c>
+      <c r="I49" t="n">
+        <v>19656</v>
+      </c>
+      <c r="J49" t="n">
         <v>19523</v>
       </c>
     </row>
     <row r="50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B50" t="n">
+        <v>22729</v>
+      </c>
+      <c r="C50" t="n">
+        <v>22657</v>
+      </c>
+      <c r="D50" t="n">
+        <v>22600</v>
+      </c>
+      <c r="E50" t="n">
+        <v>22471</v>
+      </c>
+      <c r="F50" t="n">
+        <v>22597</v>
+      </c>
+      <c r="G50" t="n">
+        <v>22975</v>
+      </c>
+      <c r="H50" t="n">
+        <v>23377</v>
+      </c>
+      <c r="I50" t="n">
+        <v>23945</v>
+      </c>
+      <c r="J50" t="n">
         <v>24064</v>
       </c>
     </row>
     <row r="51" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B51" t="n">
+        <v>6681</v>
+      </c>
+      <c r="C51" t="n">
+        <v>6826</v>
+      </c>
+      <c r="D51" t="n">
+        <v>7070</v>
+      </c>
+      <c r="E51" t="n">
+        <v>6824</v>
+      </c>
+      <c r="F51" t="n">
+        <v>6896</v>
+      </c>
+      <c r="G51" t="n">
+        <v>7118</v>
+      </c>
+      <c r="H51" t="n">
+        <v>7162</v>
+      </c>
+      <c r="I51" t="n">
+        <v>7092</v>
+      </c>
+      <c r="J51" t="n">
         <v>6775</v>
       </c>
     </row>
     <row r="52" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B52" t="n">
+        <v>2112</v>
+      </c>
+      <c r="C52" t="n">
+        <v>2183</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2204</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2310</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2383</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2424</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2374</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2473</v>
+      </c>
+      <c r="J52" t="n">
         <v>2543</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>